<commit_message>
fixed sugarbeet naming issues
</commit_message>
<xml_diff>
--- a/data/crops/crop_residue_data.xlsx
+++ b/data/crops/crop_residue_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/Ecoregions CFs/data/crops/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="40" documentId="8_{9BD4F013-961F-47EC-97FA-9734F9CC6039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD420D6E-47E9-4E85-A249-DE3352C786F9}"/>
@@ -218,7 +218,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -290,10 +290,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,7 +633,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E18FF19-B577-46F9-9040-D4A5BE97D3A9}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>